<commit_message>
do:delete user now delete history
</commit_message>
<xml_diff>
--- a/file/template_sampel.xlsx
+++ b/file/template_sampel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Koding\Project\Skripskuy\Back\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0131CF39-A65E-4132-BB80-F23BE71CEF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A430059-75E3-4D81-80C5-3AF25A1C6C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A1FBF7C8-61F9-42CA-B003-A907D1E1BB99}"/>
   </bookViews>
@@ -624,7 +624,7 @@
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -709,10 +709,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>21</v>
@@ -821,10 +821,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
do:penyesuaian dengan database berupa pergantian kolom id_x dengan nama_x di tabel dokumen, dan membuat validasi isian file 'missing-data' pada API upload
</commit_message>
<xml_diff>
--- a/file/template_sampel.xlsx
+++ b/file/template_sampel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Koding\Project\Skripskuy\Back\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A430059-75E3-4D81-80C5-3AF25A1C6C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4254EA-2789-41AB-8955-7574956CD796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A1FBF7C8-61F9-42CA-B003-A907D1E1BB99}"/>
+    <workbookView xWindow="3624" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{A1FBF7C8-61F9-42CA-B003-A907D1E1BB99}"/>
   </bookViews>
   <sheets>
     <sheet name="Lembar1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="62">
   <si>
     <t>No</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>SLS</t>
+  </si>
+  <si>
+    <t>010</t>
   </si>
 </sst>
 </file>
@@ -624,7 +627,7 @@
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -709,7 +712,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>35</v>
@@ -767,7 +770,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>36</v>
@@ -821,7 +824,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>36</v>

</xml_diff>